<commit_message>
Updated STIX_Package version numbers in example profile.
</commit_message>
<xml_diff>
--- a/examples/stix/Example_STIX_Profile.xlsx
+++ b/examples/stix/Example_STIX_Profile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="680" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -404,9 +404,6 @@
     <t>stix:STIXPackageVersionEnum</t>
   </si>
   <si>
-    <t>1.0.1, 1.1, 1.1.1</t>
-  </si>
-  <si>
     <t>TTPsType</t>
   </si>
   <si>
@@ -951,6 +948,9 @@
   </si>
   <si>
     <t>Win Filemapping Object</t>
+  </si>
+  <si>
+    <t>1.0.1, 1.1, 1.1.1,1.2</t>
   </si>
 </sst>
 </file>
@@ -2769,27 +2769,27 @@
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>216</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>217</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>218</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>219</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2799,7 +2799,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2809,37 +2809,37 @@
         <v>14</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2847,37 +2847,37 @@
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>225</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>226</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -2887,7 +2887,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2897,7 +2897,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2907,7 +2907,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -2917,7 +2917,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -2927,7 +2927,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -2937,7 +2937,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2947,7 +2947,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2957,143 +2957,143 @@
         <v>17</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3101,47 +3101,47 @@
         <v>24</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3149,79 +3149,79 @@
         <v>30</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3229,159 +3229,159 @@
         <v>34</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3389,63 +3389,63 @@
         <v>32</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
@@ -3453,47 +3453,47 @@
         <v>27</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
@@ -3501,143 +3501,143 @@
         <v>37</v>
       </c>
       <c r="B89" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B100" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
@@ -3645,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3653,23 +3653,23 @@
         <v>4</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3677,7 +3677,7 @@
         <v>6</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3685,15 +3685,15 @@
         <v>8</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>11</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3709,7 +3709,7 @@
         <v>13</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>16</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3725,7 +3725,7 @@
         <v>18</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>20</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
         <v>21</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,7 @@
         <v>22</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3757,7 +3757,7 @@
         <v>23</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3765,15 +3765,15 @@
         <v>25</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3781,7 +3781,7 @@
         <v>26</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3789,7 +3789,7 @@
         <v>28</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>29</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
         <v>31</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
         <v>33</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3821,23 +3821,23 @@
         <v>35</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3845,7 +3845,7 @@
         <v>36</v>
       </c>
       <c r="B132" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3853,7 +3853,7 @@
         <v>38</v>
       </c>
       <c r="B133" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3861,7 +3861,7 @@
         <v>39</v>
       </c>
       <c r="B134" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3869,7 +3869,7 @@
         <v>40</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>41</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3885,7 +3885,7 @@
         <v>42</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3893,7 +3893,7 @@
         <v>43</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3901,7 +3901,7 @@
         <v>44</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>45</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
         <v>46</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>47</v>
       </c>
       <c r="B142" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3933,15 +3933,15 @@
         <v>48</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
       <c r="B145" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3957,7 +3957,7 @@
         <v>50</v>
       </c>
       <c r="B146" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3965,7 +3965,7 @@
         <v>51</v>
       </c>
       <c r="B147" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3973,15 +3973,15 @@
         <v>52</v>
       </c>
       <c r="B148" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B149" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
         <v>53</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -3997,7 +3997,7 @@
         <v>54</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>55</v>
       </c>
       <c r="B152" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4013,15 +4013,15 @@
         <v>56</v>
       </c>
       <c r="B153" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B154" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4029,7 +4029,7 @@
         <v>57</v>
       </c>
       <c r="B155" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4037,7 +4037,7 @@
         <v>58</v>
       </c>
       <c r="B156" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
         <v>59</v>
       </c>
       <c r="B157" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>60</v>
       </c>
       <c r="B158" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>61</v>
       </c>
       <c r="B159" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>62</v>
       </c>
       <c r="B160" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
         <v>63</v>
       </c>
       <c r="B161" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4085,7 +4085,7 @@
         <v>64</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4093,7 +4093,7 @@
         <v>65</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>66</v>
       </c>
       <c r="B164" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4109,7 +4109,7 @@
         <v>67</v>
       </c>
       <c r="B165" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4117,7 +4117,7 @@
         <v>68</v>
       </c>
       <c r="B166" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4125,7 +4125,7 @@
         <v>69</v>
       </c>
       <c r="B167" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4133,7 +4133,7 @@
         <v>70</v>
       </c>
       <c r="B168" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
         <v>71</v>
       </c>
       <c r="B169" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>72</v>
       </c>
       <c r="B170" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4157,15 +4157,15 @@
         <v>73</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B172" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
         <v>74</v>
       </c>
       <c r="B173" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4181,7 +4181,7 @@
         <v>75</v>
       </c>
       <c r="B174" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4189,7 +4189,7 @@
         <v>76</v>
       </c>
       <c r="B175" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4197,7 +4197,7 @@
         <v>77</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4205,7 +4205,7 @@
         <v>78</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4213,7 +4213,7 @@
         <v>79</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>80</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4229,7 +4229,7 @@
         <v>81</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4237,7 +4237,7 @@
         <v>82</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4245,7 +4245,7 @@
         <v>83</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>84</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>85</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4269,7 +4269,7 @@
         <v>86</v>
       </c>
       <c r="B185" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4277,7 +4277,7 @@
         <v>87</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4285,7 +4285,7 @@
         <v>88</v>
       </c>
       <c r="B187" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4293,7 +4293,7 @@
         <v>89</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4301,7 +4301,7 @@
         <v>90</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4309,7 +4309,7 @@
         <v>91</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>92</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4325,7 +4325,7 @@
         <v>93</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4333,7 +4333,7 @@
         <v>94</v>
       </c>
       <c r="B193" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -4341,15 +4341,15 @@
         <v>95</v>
       </c>
       <c r="B194" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4827,7 +4827,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,7 +4874,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
@@ -4888,7 +4888,7 @@
         <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
         <v>105</v>
@@ -4902,7 +4902,7 @@
         <v>106</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
         <v>107</v>
@@ -4916,7 +4916,7 @@
         <v>108</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>109</v>
@@ -4930,7 +4930,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C7" t="s">
         <v>111</v>
@@ -4944,7 +4944,7 @@
         <v>112</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
@@ -4958,7 +4958,7 @@
         <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
@@ -4972,7 +4972,7 @@
         <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>117</v>
@@ -4986,7 +4986,7 @@
         <v>118</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
         <v>119</v>
@@ -5000,7 +5000,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
         <v>121</v>
@@ -5014,7 +5014,7 @@
         <v>122</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C13" t="s">
         <v>121</v>
@@ -5028,20 +5028,20 @@
         <v>123</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5" t="s">
-        <v>125</v>
+        <v>307</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -5054,10 +5054,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -5111,7 +5111,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5121,13 +5121,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5135,31 +5135,31 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5167,13 +5167,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5181,13 +5181,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5251,13 +5251,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -5273,7 +5273,7 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -5305,27 +5305,27 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" t="s">
         <v>209</v>
-      </c>
-      <c r="B4" t="s">
-        <v>219</v>
-      </c>
-      <c r="E4" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5373,45 +5373,45 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>220</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5464,7 +5464,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -5472,7 +5472,7 @@
         <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
@@ -5483,7 +5483,7 @@
         <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
         <v>121</v>
@@ -5491,13 +5491,13 @@
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -5505,43 +5505,43 @@
         <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
         <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
         <v>143</v>
-      </c>
-      <c r="B9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -5549,131 +5549,131 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" t="s">
         <v>148</v>
-      </c>
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
-      <c r="C12" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" t="s">
         <v>150</v>
-      </c>
-      <c r="B13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C13" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" t="s">
         <v>152</v>
-      </c>
-      <c r="B14" t="s">
-        <v>223</v>
-      </c>
-      <c r="C14" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" t="s">
         <v>154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C15" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" t="s">
         <v>156</v>
-      </c>
-      <c r="B16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
         <v>137</v>
-      </c>
-      <c r="B17" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" t="s">
         <v>158</v>
-      </c>
-      <c r="B18" t="s">
-        <v>220</v>
-      </c>
-      <c r="C18" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" t="s">
         <v>160</v>
-      </c>
-      <c r="B19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" t="s">
         <v>162</v>
-      </c>
-      <c r="B20" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -5681,40 +5681,40 @@
         <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" t="s">
         <v>166</v>
-      </c>
-      <c r="B23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C23" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" t="s">
         <v>169</v>
       </c>
-      <c r="B25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>170</v>
-      </c>
-      <c r="D25" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5743,10 +5743,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="E1" s="2"/>
     </row>
@@ -5756,7 +5756,7 @@
         <v>http://www.w3.org/2001/XMLSchema-instance</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -5767,7 +5767,7 @@
         <v>http://stix.mitre.org/stix-1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -5778,7 +5778,7 @@
         <v>http://stix.mitre.org/common-1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -5789,65 +5789,65 @@
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -5870,7 +5870,7 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -5884,13 +5884,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="E1" s="2"/>
     </row>
@@ -5899,21 +5899,21 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>189</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5921,76 +5921,76 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" t="s">
         <v>199</v>
-      </c>
-      <c r="B8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
         <v>204</v>
       </c>
-      <c r="B9" t="s">
-        <v>205</v>
-      </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" t="s">
         <v>211</v>
-      </c>
-      <c r="C10" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified example profile to disallow now deprecated STIX_Header fields.
</commit_message>
<xml_diff>
--- a/examples/stix/Example_STIX_Profile.xlsx
+++ b/examples/stix/Example_STIX_Profile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="680" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -4826,8 +4826,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,7 +4874,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
@@ -5077,7 +5077,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5124,7 +5124,7 @@
         <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>129</v>
@@ -5138,7 +5138,7 @@
         <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>131</v>
@@ -5870,7 +5870,7 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>